<commit_message>
atualizado sql versao BCB
</commit_message>
<xml_diff>
--- a/sql/SQL visualização/valida resultados.xlsx
+++ b/sql/SQL visualização/valida resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>VF</t>
   </si>
@@ -38,6 +38,9 @@
     <t>deposito</t>
   </si>
   <si>
+    <t>https://www3.bcb.gov.br/CALCIDADAO/publico/exibirMetodologiaAplicacaoDepositosRegulares.do?method=exibirMetodologiaAplicacaoDepositosRegulares</t>
+  </si>
+  <si>
     <t>VP*(1+taxa)^periodo</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
   </si>
   <si>
     <t>rendimento total</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
 </sst>
 </file>
@@ -70,11 +76,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,6 +97,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,8 +148,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,7 +181,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -201,7 +219,7 @@
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">LOG($B$1/$B$2)/LOG(1+$B$3)</f>
-        <v>15.932637544624</v>
+        <v>9.57859403981317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -209,7 +227,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.006</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,470 +246,481 @@
         <v>100</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D9</f>
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D9)-1)/$B$3)</f>
-        <v>100.6</v>
-      </c>
-      <c r="F9" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="F9" s="2" t="n">
         <f aca="false">E9+C9</f>
-        <v>1106.6</v>
-      </c>
-      <c r="G9" s="1" t="n">
+        <v>1111</v>
+      </c>
+      <c r="G9" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D9)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D9-1))-1)/$B$3)-$B$5</f>
-        <v>0.60000000000008</v>
-      </c>
-      <c r="H9" s="1" t="n">
+        <v>1.00000000000009</v>
+      </c>
+      <c r="H9" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D9 - $B$2*(1+$B$3)^($D9-1)</f>
-        <v>6</v>
-      </c>
-      <c r="I9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <f aca="false">H9+G9</f>
-        <v>6.60000000000008</v>
+        <v>11.0000000000001</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D10</f>
-        <v>1012.036</v>
+        <v>1020.1</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D10)-1)/$B$3)</f>
-        <v>201.803599999999</v>
-      </c>
-      <c r="F10" s="1" t="n">
+        <v>203.01</v>
+      </c>
+      <c r="F10" s="2" t="n">
         <f aca="false">E10+C10</f>
-        <v>1213.8396</v>
-      </c>
-      <c r="G10" s="1" t="n">
+        <v>1223.11</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D10)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D10-1))-1)/$B$3)-$B$5</f>
-        <v>1.20359999999883</v>
-      </c>
-      <c r="H10" s="1" t="n">
+        <v>2.00999999999999</v>
+      </c>
+      <c r="H10" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D10 - $B$2*(1+$B$3)^($D10-1)</f>
-        <v>6.03599999999994</v>
-      </c>
-      <c r="I10" s="1" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="I10" s="2" t="n">
         <f aca="false">H10+G10</f>
-        <v>7.23959999999877</v>
+        <v>12.11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D11</f>
-        <v>1018.108216</v>
+        <v>1030.301</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D11)-1)/$B$3)</f>
-        <v>303.614421600002</v>
-      </c>
-      <c r="F11" s="1" t="n">
+        <v>306.040100000001</v>
+      </c>
+      <c r="F11" s="2" t="n">
         <f aca="false">E11+C11</f>
-        <v>1321.7226376</v>
-      </c>
-      <c r="G11" s="1" t="n">
+        <v>1336.3411</v>
+      </c>
+      <c r="G11" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D11)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D11-1))-1)/$B$3)-$B$5</f>
-        <v>1.8108216000031</v>
-      </c>
-      <c r="H11" s="1" t="n">
+        <v>3.03010000000128</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D11 - $B$2*(1+$B$3)^($D11-1)</f>
-        <v>6.07221600000014</v>
-      </c>
-      <c r="I11" s="1" t="n">
+        <v>10.2010000000001</v>
+      </c>
+      <c r="I11" s="2" t="n">
         <f aca="false">H11+G11</f>
-        <v>7.88303760000323</v>
+        <v>13.2311000000014</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D12</f>
-        <v>1024.216865296</v>
+        <v>1040.60401</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D12)-1)/$B$3)</f>
-        <v>406.0361081296</v>
-      </c>
-      <c r="F12" s="1" t="n">
+        <v>410.100501</v>
+      </c>
+      <c r="F12" s="2" t="n">
         <f aca="false">E12+C12</f>
-        <v>1430.2529734256</v>
-      </c>
-      <c r="G12" s="1" t="n">
+        <v>1450.704511</v>
+      </c>
+      <c r="G12" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D12)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D12-1))-1)/$B$3)-$B$5</f>
-        <v>2.42168652959765</v>
-      </c>
-      <c r="H12" s="1" t="n">
+        <v>4.06040099999888</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D12 - $B$2*(1+$B$3)^($D12-1)</f>
-        <v>6.10864929599984</v>
-      </c>
-      <c r="I12" s="1" t="n">
+        <v>10.3030099999999</v>
+      </c>
+      <c r="I12" s="2" t="n">
         <f aca="false">H12+G12</f>
-        <v>8.53033582559749</v>
+        <v>14.3634109999987</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D13</f>
-        <v>1030.36216648778</v>
+        <v>1051.0100501</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D13)-1)/$B$3)</f>
-        <v>509.072324778378</v>
-      </c>
-      <c r="F13" s="1" t="n">
+        <v>515.201506010002</v>
+      </c>
+      <c r="F13" s="2" t="n">
         <f aca="false">E13+C13</f>
-        <v>1539.43449126615</v>
-      </c>
-      <c r="G13" s="1" t="n">
+        <v>1566.21155611</v>
+      </c>
+      <c r="G13" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D13)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D13-1))-1)/$B$3)-$B$5</f>
-        <v>3.03621664877807</v>
-      </c>
-      <c r="H13" s="1" t="n">
+        <v>5.10100501000125</v>
+      </c>
+      <c r="H13" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D13 - $B$2*(1+$B$3)^($D13-1)</f>
-        <v>6.14530119177607</v>
-      </c>
-      <c r="I13" s="1" t="n">
+        <v>10.4060401000002</v>
+      </c>
+      <c r="I13" s="2" t="n">
         <f aca="false">H13+G13</f>
-        <v>9.18151784055414</v>
+        <v>15.5070451100014</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D14</f>
-        <v>1036.5443394867</v>
+        <v>1061.520150601</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D14)-1)/$B$3)</f>
-        <v>612.726758727048</v>
-      </c>
-      <c r="F14" s="1" t="n">
+        <v>621.353521070101</v>
+      </c>
+      <c r="F14" s="2" t="n">
         <f aca="false">E14+C14</f>
-        <v>1649.27109821375</v>
-      </c>
-      <c r="G14" s="1" t="n">
+        <v>1682.8736716711</v>
+      </c>
+      <c r="G14" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D14)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D14-1))-1)/$B$3)-$B$5</f>
-        <v>3.65443394867009</v>
-      </c>
-      <c r="H14" s="1" t="n">
+        <v>6.15201506009987</v>
+      </c>
+      <c r="H14" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D14 - $B$2*(1+$B$3)^($D14-1)</f>
-        <v>6.18217299892672</v>
-      </c>
-      <c r="I14" s="1" t="n">
+        <v>10.5101005009999</v>
+      </c>
+      <c r="I14" s="2" t="n">
         <f aca="false">H14+G14</f>
-        <v>9.83660694759681</v>
+        <v>16.6621155610998</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1" t="n">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D15</f>
-        <v>1042.76360552362</v>
+        <v>1072.13535210701</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D15)-1)/$B$3)</f>
-        <v>717.003119279411</v>
-      </c>
-      <c r="F15" s="1" t="n">
+        <v>728.567056280802</v>
+      </c>
+      <c r="F15" s="2" t="n">
         <f aca="false">E15+C15</f>
-        <v>1759.76672480303</v>
-      </c>
-      <c r="G15" s="1" t="n">
+        <v>1800.70240838781</v>
+      </c>
+      <c r="G15" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D15)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D15-1))-1)/$B$3)-$B$5</f>
-        <v>4.2763605523628</v>
-      </c>
-      <c r="H15" s="1" t="n">
+        <v>7.21353521070023</v>
+      </c>
+      <c r="H15" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D15 - $B$2*(1+$B$3)^($D15-1)</f>
-        <v>6.21926603692009</v>
-      </c>
-      <c r="I15" s="1" t="n">
+        <v>10.61520150601</v>
+      </c>
+      <c r="I15" s="2" t="n">
         <f aca="false">H15+G15</f>
-        <v>10.4956265892829</v>
+        <v>17.8287367167102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D16</f>
-        <v>1049.02018715676</v>
+        <v>1082.85670562808</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D16)-1)/$B$3)</f>
-        <v>821.905137995086</v>
-      </c>
-      <c r="F16" s="1" t="n">
+        <v>836.85272684361</v>
+      </c>
+      <c r="F16" s="2" t="n">
         <f aca="false">E16+C16</f>
-        <v>1870.92532515185</v>
-      </c>
-      <c r="G16" s="1" t="n">
+        <v>1919.70943247169</v>
+      </c>
+      <c r="G16" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D16)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D16-1))-1)/$B$3)-$B$5</f>
-        <v>4.9020187156757</v>
-      </c>
-      <c r="H16" s="1" t="n">
+        <v>8.28567056280861</v>
+      </c>
+      <c r="H16" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D16 - $B$2*(1+$B$3)^($D16-1)</f>
-        <v>6.25658163314188</v>
-      </c>
-      <c r="I16" s="1" t="n">
+        <v>10.7213535210701</v>
+      </c>
+      <c r="I16" s="2" t="n">
         <f aca="false">H16+G16</f>
-        <v>11.1586003488176</v>
+        <v>19.0070240838787</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D17</f>
-        <v>1055.31430827971</v>
+        <v>1093.68527268436</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D17)-1)/$B$3)</f>
-        <v>927.436568823057</v>
-      </c>
-      <c r="F17" s="1" t="n">
+        <v>946.221254112045</v>
+      </c>
+      <c r="F17" s="2" t="n">
         <f aca="false">E17+C17</f>
-        <v>1982.75087710276</v>
-      </c>
-      <c r="G17" s="1" t="n">
+        <v>2039.90652679641</v>
+      </c>
+      <c r="G17" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D17)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D17-1))-1)/$B$3)-$B$5</f>
-        <v>5.53143082797055</v>
-      </c>
-      <c r="H17" s="1" t="n">
+        <v>9.36852726843472</v>
+      </c>
+      <c r="H17" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D17 - $B$2*(1+$B$3)^($D17-1)</f>
-        <v>6.2941211229404</v>
-      </c>
-      <c r="I17" s="1" t="n">
+        <v>10.8285670562807</v>
+      </c>
+      <c r="I17" s="2" t="n">
         <f aca="false">H17+G17</f>
-        <v>11.8255519509109</v>
+        <v>20.1970943247154</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D18</f>
-        <v>1061.64619412938</v>
+        <v>1104.6221254112</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D18)-1)/$B$3)</f>
-        <v>1033.601188236</v>
-      </c>
-      <c r="F18" s="1" t="n">
+        <v>1056.68346665317</v>
+      </c>
+      <c r="F18" s="2" t="n">
         <f aca="false">E18+C18</f>
-        <v>2095.24738236538</v>
-      </c>
-      <c r="G18" s="1" t="n">
+        <v>2161.30559206437</v>
+      </c>
+      <c r="G18" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D18)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D18-1))-1)/$B$3)-$B$5</f>
-        <v>6.16461941294051</v>
-      </c>
-      <c r="H18" s="1" t="n">
+        <v>10.4622125411207</v>
+      </c>
+      <c r="H18" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D18 - $B$2*(1+$B$3)^($D18-1)</f>
-        <v>6.33188584967843</v>
-      </c>
-      <c r="I18" s="1" t="n">
+        <v>10.9368527268437</v>
+      </c>
+      <c r="I18" s="2" t="n">
         <f aca="false">H18+G18</f>
-        <v>12.4965052626189</v>
+        <v>21.3990652679644</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D19</f>
-        <v>1068.01607129416</v>
+        <v>1115.66834666532</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D19)-1)/$B$3)</f>
-        <v>1140.40279536541</v>
-      </c>
-      <c r="F19" s="1" t="n">
+        <v>1168.2503013197</v>
+      </c>
+      <c r="F19" s="2" t="n">
         <f aca="false">E19+C19</f>
-        <v>2208.41886665957</v>
-      </c>
-      <c r="G19" s="1" t="n">
+        <v>2283.91864798501</v>
+      </c>
+      <c r="G19" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D19)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D19-1))-1)/$B$3)-$B$5</f>
-        <v>6.80160712941461</v>
-      </c>
-      <c r="H19" s="1" t="n">
+        <v>11.5668346665316</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D19 - $B$2*(1+$B$3)^($D19-1)</f>
-        <v>6.3698771647762</v>
-      </c>
-      <c r="I19" s="1" t="n">
+        <v>11.046221254112</v>
+      </c>
+      <c r="I19" s="2" t="n">
         <f aca="false">H19+G19</f>
-        <v>13.1714842941908</v>
+        <v>22.6130559206435</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D20</f>
-        <v>1074.42416772192</v>
+        <v>1126.82503013197</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D20)-1)/$B$3)</f>
-        <v>1247.84521213761</v>
-      </c>
-      <c r="F20" s="1" t="n">
+        <v>1280.93280433289</v>
+      </c>
+      <c r="F20" s="2" t="n">
         <f aca="false">E20+C20</f>
-        <v>2322.26937985953</v>
-      </c>
-      <c r="G20" s="1" t="n">
+        <v>2407.75783446486</v>
+      </c>
+      <c r="G20" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D20)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D20-1))-1)/$B$3)-$B$5</f>
-        <v>7.44241677219452</v>
-      </c>
-      <c r="H20" s="1" t="n">
+        <v>12.6825030131974</v>
+      </c>
+      <c r="H20" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D20 - $B$2*(1+$B$3)^($D20-1)</f>
-        <v>6.40809642776503</v>
-      </c>
-      <c r="I20" s="1" t="n">
+        <v>11.1566834666532</v>
+      </c>
+      <c r="I20" s="2" t="n">
         <f aca="false">H20+G20</f>
-        <v>13.8505131999596</v>
+        <v>23.8391864798507</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D21</f>
-        <v>1080.87071272826</v>
+        <v>1138.09328043329</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D21)-1)/$B$3)</f>
-        <v>1355.93228341043</v>
-      </c>
-      <c r="F21" s="1" t="n">
+        <v>1394.74213237622</v>
+      </c>
+      <c r="F21" s="2" t="n">
         <f aca="false">E21+C21</f>
-        <v>2436.80299613869</v>
-      </c>
-      <c r="G21" s="1" t="n">
+        <v>2532.83541280951</v>
+      </c>
+      <c r="G21" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D21)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D21-1))-1)/$B$3)-$B$5</f>
-        <v>8.08707127282605</v>
-      </c>
-      <c r="H21" s="1" t="n">
+        <v>13.8093280433293</v>
+      </c>
+      <c r="H21" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D21 - $B$2*(1+$B$3)^($D21-1)</f>
-        <v>6.44654500633169</v>
-      </c>
-      <c r="I21" s="1" t="n">
+        <v>11.2682503013198</v>
+      </c>
+      <c r="I21" s="2" t="n">
         <f aca="false">H21+G21</f>
-        <v>14.5336162791577</v>
+        <v>25.0775783446491</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D22</f>
-        <v>1087.35593700463</v>
+        <v>1149.47421323762</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D22)-1)/$B$3)</f>
-        <v>1464.6678771109</v>
-      </c>
-      <c r="F22" s="1" t="n">
+        <v>1509.68955369999</v>
+      </c>
+      <c r="F22" s="2" t="n">
         <f aca="false">E22+C22</f>
-        <v>2552.02381411552</v>
-      </c>
-      <c r="G22" s="1" t="n">
+        <v>2659.16376693761</v>
+      </c>
+      <c r="G22" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D22)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D22-1))-1)/$B$3)-$B$5</f>
-        <v>8.73559370046269</v>
-      </c>
-      <c r="H22" s="1" t="n">
+        <v>14.9474213237638</v>
+      </c>
+      <c r="H22" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D22 - $B$2*(1+$B$3)^($D22-1)</f>
-        <v>6.48522427636954</v>
-      </c>
-      <c r="I22" s="1" t="n">
+        <v>11.380932804333</v>
+      </c>
+      <c r="I22" s="2" t="n">
         <f aca="false">H22+G22</f>
-        <v>15.2208179768322</v>
+        <v>26.3283541280969</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D23</f>
-        <v>1093.88007262665</v>
+        <v>1160.96895537</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D23)-1)/$B$3)</f>
-        <v>1574.05588437356</v>
-      </c>
-      <c r="F23" s="1" t="n">
+        <v>1625.78644923699</v>
+      </c>
+      <c r="F23" s="2" t="n">
         <f aca="false">E23+C23</f>
-        <v>2667.93595700021</v>
-      </c>
-      <c r="G23" s="1" t="n">
+        <v>2786.75540460699</v>
+      </c>
+      <c r="G23" s="2" t="n">
         <f aca="false">($B$5)*(1+$B$3)*((((1+$B$3)^$D23)-1)/$B$3)-($B$5)*(1+$B$3)*((((1+$B$3)^($D23-1))-1)/$B$3)-$B$5</f>
-        <v>9.38800726266231</v>
-      </c>
-      <c r="H23" s="1" t="n">
+        <v>16.0968955369988</v>
+      </c>
+      <c r="H23" s="2" t="n">
         <f aca="false">$B$2*(1+$B$3)^$D23 - $B$2*(1+$B$3)^($D23-1)</f>
-        <v>6.52413562202764</v>
-      </c>
-      <c r="I23" s="1" t="n">
+        <v>11.4947421323761</v>
+      </c>
+      <c r="I23" s="2" t="n">
         <f aca="false">H23+G23</f>
-        <v>15.91214288469</v>
+        <v>27.5916376693749</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" display="https://www3.bcb.gov.br/CALCIDADAO/publico/exibirMetodologiaAplicacaoDepositosRegulares.do?method=exibirMetodologiaAplicacaoDepositosRegulares"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>